<commit_message>
Probando en Diciembre 2025
</commit_message>
<xml_diff>
--- a/resultados_evaluacion/reporte_evaluacion.xlsx
+++ b/resultados_evaluacion/reporte_evaluacion.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programas propios\Python\API_CompararTextos\resultados_evaluacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A16A810-5A45-4617-8778-3ECBC3B0E036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57475A32-051D-473E-A70A-801A48FECC92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen Ejecutivo" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
     <t>Tiempo Respuesta Promedio (s)</t>
   </si>
   <si>
-    <t>3.36</t>
+    <t>7.16</t>
   </si>
   <si>
     <t>Resumen de las métricas clave de evaluación</t>
@@ -83,7 +83,7 @@
     <t>Umbral de similitud: 0.7</t>
   </si>
   <si>
-    <t>Fecha generación: 2025-05-21 23:19:46</t>
+    <t>Fecha generación: 2025-05-22 15:43:10</t>
   </si>
   <si>
     <t>Métricas Similitud</t>
@@ -182,64 +182,64 @@
     <t>Tipo Error</t>
   </si>
   <si>
+    <t>0_demo.json</t>
+  </si>
+  <si>
+    <t>Similar</t>
+  </si>
+  <si>
+    <t>Sí</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
     <t>10_sistemas_operativos.json</t>
   </si>
   <si>
     <t>No Similar</t>
   </si>
   <si>
-    <t>Similar</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Falso Negativo</t>
   </si>
   <si>
+    <t>11_ingenieria_economica.json</t>
+  </si>
+  <si>
     <t>12_taller_de_proyectos_1.json</t>
   </si>
   <si>
-    <t>Sí</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>0_demo.json</t>
-  </si>
-  <si>
-    <t>11_ingenieria_economica.json</t>
+    <t>13_taller_de_proyectos_2.json</t>
+  </si>
+  <si>
+    <t>1_redes_computadoras.json</t>
   </si>
   <si>
     <t>3_auditoría_sistemas.json</t>
   </si>
   <si>
-    <t>13_taller_de_proyectos_2.json</t>
-  </si>
-  <si>
-    <t>1_redes_computadoras.json</t>
+    <t>5_estructura_de_datos.json</t>
+  </si>
+  <si>
+    <t>6_matematica_discreta.json</t>
   </si>
   <si>
     <t>2_base_de_datos.json</t>
   </si>
   <si>
+    <t>4_arquitectura_computador.json</t>
+  </si>
+  <si>
     <t>7_ecuaciones_diferenciales.json</t>
   </si>
   <si>
-    <t>5_estructura_de_datos.json</t>
-  </si>
-  <si>
-    <t>6_matematica_discreta.json</t>
-  </si>
-  <si>
-    <t>4_arquitectura_computador.json</t>
+    <t>8_investigacion_operativa.json</t>
   </si>
   <si>
     <t>9_sistemas_digitales.json</t>
-  </si>
-  <si>
-    <t>8_investigacion_operativa.json</t>
   </si>
   <si>
     <t>Comparación detallada entre predicciones del modelo y golden standard</t>
@@ -466,7 +466,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -478,6 +478,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -608,7 +611,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6787-421F-A84C-76CA508DB30E}"/>
+              <c16:uniqueId val="{00000000-A2D3-46C8-85FA-BBCBA36DA090}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -814,7 +817,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>0.75709245509334988</c:v>
+                  <c:v>0.75709245509334977</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.7472309069335461</c:v>
@@ -835,10 +838,10 @@
                   <c:v>2.0173307003516572E-3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.4914704722970822E-2</c:v>
+                  <c:v>4.4914704722970808E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.63718105832317884</c:v>
+                  <c:v>0.63718105832317895</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>0.8571428571428571</c:v>
@@ -857,7 +860,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-6434-47FF-9E8D-7C78248E1456}"/>
+              <c16:uniqueId val="{00000000-6DC1-46A0-BDED-333E74DDCA85}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -974,6 +977,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-PE"/>
               <a:t>Distribución de Similitudes</a:t>
             </a:r>
           </a:p>
@@ -1045,7 +1049,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-4389-4F34-8366-8BBFA547C6A5}"/>
+              <c16:uniqueId val="{00000000-3A75-4CBF-B15E-4D9BA807A232}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1106,7 +1110,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-4389-4F34-8366-8BBFA547C6A5}"/>
+              <c16:uniqueId val="{00000001-3A75-4CBF-B15E-4D9BA807A232}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1138,7 +1142,7 @@
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1173,6 +1177,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-PE"/>
                   <a:t>Porcentaje</a:t>
                 </a:r>
               </a:p>
@@ -1222,6 +1227,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-PE"/>
               <a:t>Distribución de Tipos de Error</a:t>
             </a:r>
           </a:p>
@@ -1293,7 +1299,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B3E4-4D99-A82C-22C259026711}"/>
+              <c16:uniqueId val="{00000000-A913-4F88-9277-4B53B7A16A53}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1354,7 +1360,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-B3E4-4D99-A82C-22C259026711}"/>
+              <c16:uniqueId val="{00000001-A913-4F88-9277-4B53B7A16A53}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1386,7 +1392,7 @@
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1421,6 +1427,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-PE"/>
                   <a:t>Porcentaje</a:t>
                 </a:r>
               </a:p>
@@ -1470,6 +1477,7 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
+              <a:rPr lang="es-PE"/>
               <a:t>Evolución Similitud por Archivo</a:t>
             </a:r>
           </a:p>
@@ -1511,46 +1519,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0_demo.json</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10_sistemas_operativos.json</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>11_ingenieria_economica.json</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12_taller_de_proyectos_1.json</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0_demo.json</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11_ingenieria_economica.json</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>13_taller_de_proyectos_2.json</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1_redes_computadoras.json</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3_auditoría_sistemas.json</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>13_taller_de_proyectos_2.json</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1_redes_computadoras.json</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>5_estructura_de_datos.json</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6_matematica_discreta.json</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2_base_de_datos.json</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>4_arquitectura_computador.json</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>7_ecuaciones_diferenciales.json</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>5_estructura_de_datos.json</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6_matematica_discreta.json</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4_arquitectura_computador.json</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>8_investigacion_operativa.json</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9_sistemas_digitales.json</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8_investigacion_operativa.json</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1609,7 +1617,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7B44-415F-B41E-54C7941CEF79}"/>
+              <c16:uniqueId val="{00000000-1C11-4CB1-8970-4CEE90D2D796}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1641,46 +1649,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0_demo.json</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10_sistemas_operativos.json</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>11_ingenieria_economica.json</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12_taller_de_proyectos_1.json</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0_demo.json</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11_ingenieria_economica.json</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>13_taller_de_proyectos_2.json</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1_redes_computadoras.json</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3_auditoría_sistemas.json</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>13_taller_de_proyectos_2.json</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1_redes_computadoras.json</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>5_estructura_de_datos.json</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6_matematica_discreta.json</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2_base_de_datos.json</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>4_arquitectura_computador.json</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>7_ecuaciones_diferenciales.json</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>5_estructura_de_datos.json</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6_matematica_discreta.json</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4_arquitectura_computador.json</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>8_investigacion_operativa.json</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9_sistemas_digitales.json</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8_investigacion_operativa.json</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1692,46 +1700,46 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
-                  <c:v>2.595370769500732</c:v>
+                  <c:v>3.5542223453521729</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.600854873657227</c:v>
+                  <c:v>4.3511195182800293</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6018660068511958</c:v>
+                  <c:v>4.5891110897064209</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.6008567810058589</c:v>
+                  <c:v>4.9205563068389893</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8211498260498051</c:v>
+                  <c:v>2.7988286018371582</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.9967186450958252</c:v>
+                  <c:v>3.7397370338439941</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.0274679660797119</c:v>
+                  <c:v>8.2300188541412354</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4.0721776485443124</c:v>
+                  <c:v>13.553435564041139</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.8675799369812012</c:v>
+                  <c:v>9.9214291572570801</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4.0175836086273193</c:v>
+                  <c:v>18.355663776397709</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3.987694263458252</c:v>
+                  <c:v>17.413506507873539</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.3103392124176034</c:v>
+                  <c:v>2.891057968139648</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.238385677337646</c:v>
+                  <c:v>2.892987966537476</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.296442031860352</c:v>
+                  <c:v>2.9773752689361568</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,7 +1747,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7B44-415F-B41E-54C7941CEF79}"/>
+              <c16:uniqueId val="{00000001-1C11-4CB1-8970-4CEE90D2D796}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1771,46 +1779,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0_demo.json</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10_sistemas_operativos.json</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>11_ingenieria_economica.json</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12_taller_de_proyectos_1.json</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0_demo.json</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11_ingenieria_economica.json</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>13_taller_de_proyectos_2.json</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1_redes_computadoras.json</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3_auditoría_sistemas.json</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>13_taller_de_proyectos_2.json</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1_redes_computadoras.json</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>5_estructura_de_datos.json</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6_matematica_discreta.json</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2_base_de_datos.json</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>4_arquitectura_computador.json</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>7_ecuaciones_diferenciales.json</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>5_estructura_de_datos.json</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6_matematica_discreta.json</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4_arquitectura_computador.json</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>8_investigacion_operativa.json</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9_sistemas_digitales.json</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8_investigacion_operativa.json</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1822,46 +1830,46 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>1.000000027418136</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.68509304702281959</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>0.68147463917732243</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.75970676183700558</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.000000027418136</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.68147463917732243</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.77654744505882256</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.74033935010433194</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.75292744398117062</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.77654744505882256</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.74033935010433194</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.68647099554538726</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.76516832530498502</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.75246476262807849</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>0.71983874142169957</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.80050379097461699</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.68647099554538726</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.76516832530498502</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.71983874142169957</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>0.74199705123901372</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.73676198959350581</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.74199705123901372</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1869,7 +1877,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-7B44-415F-B41E-54C7941CEF79}"/>
+              <c16:uniqueId val="{00000002-1C11-4CB1-8970-4CEE90D2D796}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1901,46 +1909,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0_demo.json</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10_sistemas_operativos.json</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>11_ingenieria_economica.json</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12_taller_de_proyectos_1.json</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0_demo.json</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11_ingenieria_economica.json</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>13_taller_de_proyectos_2.json</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1_redes_computadoras.json</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3_auditoría_sistemas.json</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>13_taller_de_proyectos_2.json</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1_redes_computadoras.json</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>5_estructura_de_datos.json</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6_matematica_discreta.json</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2_base_de_datos.json</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>4_arquitectura_computador.json</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>7_ecuaciones_diferenciales.json</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>5_estructura_de_datos.json</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6_matematica_discreta.json</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4_arquitectura_computador.json</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>8_investigacion_operativa.json</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9_sistemas_digitales.json</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8_investigacion_operativa.json</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1964,10 +1972,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -1976,7 +1984,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.75</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>1</c:v>
@@ -1985,13 +1993,13 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="11">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.75</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.75</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1999,7 +2007,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-7B44-415F-B41E-54C7941CEF79}"/>
+              <c16:uniqueId val="{00000003-1C11-4CB1-8970-4CEE90D2D796}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2031,46 +2039,46 @@
               <c:strCache>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0_demo.json</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>10_sistemas_operativos.json</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>11_ingenieria_economica.json</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>12_taller_de_proyectos_1.json</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0_demo.json</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11_ingenieria_economica.json</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>13_taller_de_proyectos_2.json</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1_redes_computadoras.json</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>3_auditoría_sistemas.json</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>13_taller_de_proyectos_2.json</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1_redes_computadoras.json</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>5_estructura_de_datos.json</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>6_matematica_discreta.json</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>2_base_de_datos.json</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>4_arquitectura_computador.json</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>7_ecuaciones_diferenciales.json</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>5_estructura_de_datos.json</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>6_matematica_discreta.json</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4_arquitectura_computador.json</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>8_investigacion_operativa.json</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>9_sistemas_digitales.json</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8_investigacion_operativa.json</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2082,46 +2090,46 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="14"/>
                 <c:pt idx="0">
+                  <c:v>0.99999993672706555</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>0.92804513378079856</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="2">
+                  <c:v>0.92245274505299124</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>0.95026059723729361</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.99999993672706555</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.92245274505299124</c:v>
-                </c:pt>
                 <c:pt idx="4">
+                  <c:v>0.97323653638405838</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96951785619506203</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.94548490063984159</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.97323653638405838</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.96951785619506203</c:v>
-                </c:pt>
                 <c:pt idx="7">
+                  <c:v>0.95844342781054226</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.92668816443314339</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.92829779530848466</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="10">
+                  <c:v>0.90114483264887002</c:v>
+                </c:pt>
+                <c:pt idx="11">
                   <c:v>0.93549767296892161</c:v>
                 </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.95844342781054226</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.92668816443314339</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.90114483264887002</c:v>
-                </c:pt>
                 <c:pt idx="12">
+                  <c:v>0.93286910756294672</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>0.93800639463781632</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.93286910756294672</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2129,7 +2137,7 @@
           <c:smooth val="1"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000004-7B44-415F-B41E-54C7941CEF79}"/>
+              <c16:uniqueId val="{00000004-1C11-4CB1-8970-4CEE90D2D796}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2161,7 +2169,7 @@
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
-                <a:endParaRPr/>
+                <a:endParaRPr lang="es-PE"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2196,6 +2204,7 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
+                  <a:rPr lang="es-PE"/>
                   <a:t>Similitud</a:t>
                 </a:r>
               </a:p>
@@ -2771,8 +2780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2878,7 +2887,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -2923,36 +2934,36 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>2.595370769500732</v>
+        <v>3.5542223453521729</v>
       </c>
       <c r="D3" s="3">
-        <v>0.68509304702281959</v>
+        <v>1.000000027418136</v>
       </c>
       <c r="E3" s="3">
         <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>0.92804513378079856</v>
+        <v>0.99999993672706555</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3">
-        <v>2.600854873657227</v>
+        <v>4.3511195182800293</v>
       </c>
       <c r="D4" s="3">
-        <v>0.75970676183700558</v>
+        <v>0.68509304702281959</v>
       </c>
       <c r="E4" s="3">
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>0.95026059723729361</v>
+        <v>0.92804513378079856</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -2963,16 +2974,16 @@
         <v>1</v>
       </c>
       <c r="C5" s="3">
-        <v>2.6018660068511958</v>
+        <v>4.5891110897064209</v>
       </c>
       <c r="D5" s="3">
-        <v>1.000000027418136</v>
+        <v>0.68147463917732243</v>
       </c>
       <c r="E5" s="3">
         <v>1</v>
       </c>
       <c r="F5" s="3">
-        <v>0.99999993672706555</v>
+        <v>0.92245274505299124</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -2983,16 +2994,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="3">
-        <v>2.6008567810058589</v>
+        <v>4.9205563068389893</v>
       </c>
       <c r="D6" s="3">
-        <v>0.68147463917732243</v>
+        <v>0.75970676183700558</v>
       </c>
       <c r="E6" s="3">
         <v>1</v>
       </c>
       <c r="F6" s="3">
-        <v>0.92245274505299124</v>
+        <v>0.95026059723729361</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -3003,16 +3014,16 @@
         <v>1</v>
       </c>
       <c r="C7" s="3">
-        <v>3.8211498260498051</v>
+        <v>2.7988286018371582</v>
       </c>
       <c r="D7" s="3">
-        <v>0.75292744398117062</v>
+        <v>0.77654744505882256</v>
       </c>
       <c r="E7" s="3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F7" s="3">
-        <v>0.94548490063984159</v>
+        <v>0.97323653638405838</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -3023,16 +3034,16 @@
         <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>3.9967186450958252</v>
+        <v>3.7397370338439941</v>
       </c>
       <c r="D8" s="3">
-        <v>0.77654744505882256</v>
+        <v>0.74033935010433194</v>
       </c>
       <c r="E8" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F8" s="3">
-        <v>0.97323653638405838</v>
+        <v>0.96951785619506203</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -3043,16 +3054,16 @@
         <v>1</v>
       </c>
       <c r="C9" s="3">
-        <v>4.0274679660797119</v>
+        <v>8.2300188541412354</v>
       </c>
       <c r="D9" s="3">
-        <v>0.74033935010433194</v>
+        <v>0.75292744398117062</v>
       </c>
       <c r="E9" s="3">
         <v>1</v>
       </c>
       <c r="F9" s="3">
-        <v>0.96951785619506203</v>
+        <v>0.94548490063984159</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -3063,16 +3074,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="3">
-        <v>4.0721776485443124</v>
+        <v>13.553435564041139</v>
       </c>
       <c r="D10" s="3">
-        <v>0.75246476262807849</v>
+        <v>0.68647099554538726</v>
       </c>
       <c r="E10" s="3">
         <v>1</v>
       </c>
       <c r="F10" s="3">
-        <v>0.92829779530848466</v>
+        <v>0.95844342781054226</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -3083,16 +3094,16 @@
         <v>1</v>
       </c>
       <c r="C11" s="3">
-        <v>3.8675799369812012</v>
+        <v>9.9214291572570801</v>
       </c>
       <c r="D11" s="3">
-        <v>0.80050379097461699</v>
+        <v>0.76516832530498502</v>
       </c>
       <c r="E11" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F11" s="3">
-        <v>0.93549767296892161</v>
+        <v>0.92668816443314339</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -3103,16 +3114,16 @@
         <v>1</v>
       </c>
       <c r="C12" s="3">
-        <v>4.0175836086273193</v>
+        <v>18.355663776397709</v>
       </c>
       <c r="D12" s="3">
-        <v>0.68647099554538726</v>
+        <v>0.75246476262807849</v>
       </c>
       <c r="E12" s="3">
         <v>1</v>
       </c>
       <c r="F12" s="3">
-        <v>0.95844342781054226</v>
+        <v>0.92829779530848466</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -3123,16 +3134,16 @@
         <v>1</v>
       </c>
       <c r="C13" s="3">
-        <v>3.987694263458252</v>
+        <v>17.413506507873539</v>
       </c>
       <c r="D13" s="3">
-        <v>0.76516832530498502</v>
+        <v>0.71983874142169957</v>
       </c>
       <c r="E13" s="3">
         <v>1</v>
       </c>
       <c r="F13" s="3">
-        <v>0.92668816443314339</v>
+        <v>0.90114483264887002</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -3143,16 +3154,16 @@
         <v>1</v>
       </c>
       <c r="C14" s="3">
-        <v>4.3103392124176034</v>
+        <v>2.891057968139648</v>
       </c>
       <c r="D14" s="3">
-        <v>0.71983874142169957</v>
+        <v>0.80050379097461699</v>
       </c>
       <c r="E14" s="3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F14" s="3">
-        <v>0.90114483264887002</v>
+        <v>0.93549767296892161</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -3163,16 +3174,16 @@
         <v>1</v>
       </c>
       <c r="C15" s="3">
-        <v>2.238385677337646</v>
+        <v>2.892987966537476</v>
       </c>
       <c r="D15" s="3">
-        <v>0.73676198959350581</v>
+        <v>0.74199705123901372</v>
       </c>
       <c r="E15" s="3">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F15" s="3">
-        <v>0.93800639463781632</v>
+        <v>0.93286910756294672</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -3183,16 +3194,16 @@
         <v>1</v>
       </c>
       <c r="C16" s="3">
-        <v>2.296442031860352</v>
+        <v>2.9773752689361568</v>
       </c>
       <c r="D16" s="3">
-        <v>0.74199705123901372</v>
+        <v>0.73676198959350581</v>
       </c>
       <c r="E16" s="3">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F16" s="3">
-        <v>0.93286910756294672</v>
+        <v>0.93800639463781632</v>
       </c>
     </row>
   </sheetData>
@@ -3208,7 +3219,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -3274,72 +3287,72 @@
         <v>50</v>
       </c>
       <c r="B3" s="3">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="D3" s="3">
-        <v>0.71143335103988647</v>
+        <v>1.00000011920929</v>
       </c>
       <c r="E3" s="3">
-        <v>0.84402710199356079</v>
+        <v>1</v>
       </c>
       <c r="F3" s="3">
-        <v>0.64430882334709172</v>
+        <v>0.99999998609224949</v>
       </c>
       <c r="G3" s="3">
-        <v>0.72493410110473633</v>
+        <v>1.00000011920929</v>
       </c>
       <c r="H3" s="3">
-        <v>0.68509304702281959</v>
+        <v>1.000000027418136</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J3" s="3">
-        <v>0.76250000000000007</v>
+        <v>1</v>
       </c>
       <c r="K3" s="3">
-        <v>7.7406952977180477E-2</v>
+        <v>2.7418136427925791E-8</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B4" s="3">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C4" s="3">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3">
-        <v>0.73033058643341064</v>
+        <v>0.71143335103988647</v>
       </c>
       <c r="E4" s="3">
-        <v>0.74509632587432861</v>
+        <v>0.84402710199356079</v>
       </c>
       <c r="F4" s="3">
-        <v>0.7661710023880004</v>
+        <v>0.64430882334709172</v>
       </c>
       <c r="G4" s="3">
-        <v>0.858237624168396</v>
+        <v>0.72493410110473633</v>
       </c>
       <c r="H4" s="3">
-        <v>0.75970676183700558</v>
+        <v>0.68509304702281959</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J4" s="3">
-        <v>0.78250000000000008</v>
+        <v>0.76250000000000007</v>
       </c>
       <c r="K4" s="3">
-        <v>2.27932381629945E-2</v>
+        <v>7.7406952977180477E-2</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>56</v>
@@ -3350,34 +3363,34 @@
         <v>58</v>
       </c>
       <c r="B5" s="3">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3">
-        <v>1.00000011920929</v>
+        <v>0.66701602935791016</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>0.77494865655899048</v>
       </c>
       <c r="F5" s="3">
-        <v>0.99999998609224949</v>
+        <v>0.65834386348724361</v>
       </c>
       <c r="G5" s="3">
-        <v>1.00000011920929</v>
+        <v>0.84438896179199219</v>
       </c>
       <c r="H5" s="3">
-        <v>1.000000027418136</v>
+        <v>0.68147463917732243</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J5" s="3">
-        <v>1</v>
+        <v>0.78</v>
       </c>
       <c r="K5" s="3">
-        <v>2.7418136427925791E-8</v>
+        <v>9.8525360822677599E-2</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>56</v>
@@ -3388,37 +3401,37 @@
         <v>59</v>
       </c>
       <c r="B6" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3">
-        <v>0.66701602935791016</v>
+        <v>0.73033058643341064</v>
       </c>
       <c r="E6" s="3">
-        <v>0.77494865655899048</v>
+        <v>0.74509632587432861</v>
       </c>
       <c r="F6" s="3">
-        <v>0.65834386348724361</v>
+        <v>0.7661710023880004</v>
       </c>
       <c r="G6" s="3">
-        <v>0.84438896179199219</v>
+        <v>0.858237624168396</v>
       </c>
       <c r="H6" s="3">
-        <v>0.68147463917732243</v>
+        <v>0.75970676183700558</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J6" s="3">
-        <v>0.78</v>
+        <v>0.78250000000000008</v>
       </c>
       <c r="K6" s="3">
-        <v>9.8525360822677599E-2</v>
+        <v>2.27932381629945E-2</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.35">
@@ -3426,37 +3439,37 @@
         <v>60</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
-        <v>0.80195152759552002</v>
+        <v>0.74603235721588135</v>
       </c>
       <c r="E7" s="3">
-        <v>0.79026275873184204</v>
+        <v>0.73444849252700806</v>
       </c>
       <c r="F7" s="3">
-        <v>0.71650513112545</v>
+        <v>0.79506991505622848</v>
       </c>
       <c r="G7" s="3">
-        <v>0.87020415067672729</v>
+        <v>0.79105114936828613</v>
       </c>
       <c r="H7" s="3">
-        <v>0.75292744398117062</v>
+        <v>0.77654744505882256</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J7" s="3">
-        <v>0.79549999999999998</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="K7" s="3">
-        <v>4.2572556018829373E-2</v>
+        <v>6.1547445058822592E-2</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.35">
@@ -3464,37 +3477,37 @@
         <v>61</v>
       </c>
       <c r="B8" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>0.74603235721588135</v>
+        <v>0.79246711730957031</v>
       </c>
       <c r="E8" s="3">
-        <v>0.73444849252700806</v>
+        <v>0.71754336357116699</v>
       </c>
       <c r="F8" s="3">
-        <v>0.79506991505622848</v>
+        <v>0.7210057020187377</v>
       </c>
       <c r="G8" s="3">
-        <v>0.79105114936828613</v>
+        <v>0.75729626417160034</v>
       </c>
       <c r="H8" s="3">
-        <v>0.77654744505882256</v>
+        <v>0.74033935010433194</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J8" s="3">
-        <v>0.71499999999999997</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="K8" s="3">
-        <v>6.1547445058822592E-2</v>
+        <v>4.4660649895668092E-2</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.35">
@@ -3502,37 +3515,37 @@
         <v>62</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
-        <v>0.79246711730957031</v>
+        <v>0.80195152759552002</v>
       </c>
       <c r="E9" s="3">
-        <v>0.71754336357116699</v>
+        <v>0.79026275873184204</v>
       </c>
       <c r="F9" s="3">
-        <v>0.7210057020187377</v>
+        <v>0.71650513112545</v>
       </c>
       <c r="G9" s="3">
-        <v>0.75729626417160034</v>
+        <v>0.87020415067672729</v>
       </c>
       <c r="H9" s="3">
-        <v>0.74033935010433194</v>
+        <v>0.75292744398117062</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J9" s="3">
-        <v>0.78500000000000003</v>
+        <v>0.79549999999999998</v>
       </c>
       <c r="K9" s="3">
-        <v>4.4660649895668092E-2</v>
+        <v>4.2572556018829373E-2</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.35">
@@ -3540,37 +3553,37 @@
         <v>63</v>
       </c>
       <c r="B10" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3">
-        <v>0.79038083553314209</v>
+        <v>0.75715744495391846</v>
       </c>
       <c r="E10" s="3">
-        <v>0.71320599317550659</v>
+        <v>0.73578143119812012</v>
       </c>
       <c r="F10" s="3">
-        <v>0.73118032068014149</v>
+        <v>0.64790996611118312</v>
       </c>
       <c r="G10" s="3">
-        <v>0.89681524038314819</v>
+        <v>0.69715023040771484</v>
       </c>
       <c r="H10" s="3">
-        <v>0.75246476262807849</v>
+        <v>0.68647099554538726</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>56</v>
       </c>
       <c r="J10" s="3">
-        <v>0.755</v>
+        <v>0.64749999999999996</v>
       </c>
       <c r="K10" s="3">
-        <v>2.5352373719215171E-3</v>
+        <v>3.8970995545387299E-2</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.35">
@@ -3578,37 +3591,37 @@
         <v>64</v>
       </c>
       <c r="B11" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3">
-        <v>0.91387432813644409</v>
+        <v>0.88264942169189453</v>
       </c>
       <c r="E11" s="3">
-        <v>0.7539750337600708</v>
+        <v>0.71406412124633789</v>
       </c>
       <c r="F11" s="3">
-        <v>0.76222538550694774</v>
+        <v>0.71884390413761134</v>
       </c>
       <c r="G11" s="3">
-        <v>0.786049485206604</v>
+        <v>0.83586430549621582</v>
       </c>
       <c r="H11" s="3">
-        <v>0.80050379097461699</v>
+        <v>0.76516832530498502</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J11" s="3">
-        <v>0.75900000000000001</v>
+        <v>0.77749999999999997</v>
       </c>
       <c r="K11" s="3">
-        <v>4.1503790974616983E-2</v>
+        <v>1.2331674695014949E-2</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.35">
@@ -3616,37 +3629,37 @@
         <v>65</v>
       </c>
       <c r="B12" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3">
-        <v>0.75715744495391846</v>
+        <v>0.79038083553314209</v>
       </c>
       <c r="E12" s="3">
-        <v>0.73578143119812012</v>
+        <v>0.71320599317550659</v>
       </c>
       <c r="F12" s="3">
-        <v>0.64790996611118312</v>
+        <v>0.73118032068014149</v>
       </c>
       <c r="G12" s="3">
-        <v>0.69715023040771484</v>
+        <v>0.89681524038314819</v>
       </c>
       <c r="H12" s="3">
-        <v>0.68647099554538726</v>
+        <v>0.75246476262807849</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J12" s="3">
-        <v>0.64749999999999996</v>
+        <v>0.755</v>
       </c>
       <c r="K12" s="3">
-        <v>3.8970995545387299E-2</v>
+        <v>2.5352373719215171E-3</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.35">
@@ -3654,37 +3667,37 @@
         <v>66</v>
       </c>
       <c r="B13" s="3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
-        <v>0.88264942169189453</v>
+        <v>0.82644057273864746</v>
       </c>
       <c r="E13" s="3">
-        <v>0.71406412124633789</v>
+        <v>0.79643505811691284</v>
       </c>
       <c r="F13" s="3">
-        <v>0.71884390413761134</v>
+        <v>0.67437954246997833</v>
       </c>
       <c r="G13" s="3">
-        <v>0.83586430549621582</v>
+        <v>0.5791473388671875</v>
       </c>
       <c r="H13" s="3">
-        <v>0.76516832530498502</v>
+        <v>0.71983874142169957</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J13" s="3">
-        <v>0.77749999999999997</v>
+        <v>0.73749999999999993</v>
       </c>
       <c r="K13" s="3">
-        <v>1.2331674695014949E-2</v>
+        <v>1.7661258578300369E-2</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.35">
@@ -3692,37 +3705,37 @@
         <v>67</v>
       </c>
       <c r="B14" s="3">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3">
-        <v>0.82644057273864746</v>
+        <v>0.91387432813644409</v>
       </c>
       <c r="E14" s="3">
-        <v>0.79643505811691284</v>
+        <v>0.7539750337600708</v>
       </c>
       <c r="F14" s="3">
-        <v>0.67437954246997833</v>
+        <v>0.76222538550694774</v>
       </c>
       <c r="G14" s="3">
-        <v>0.5791473388671875</v>
+        <v>0.786049485206604</v>
       </c>
       <c r="H14" s="3">
-        <v>0.71983874142169957</v>
+        <v>0.80050379097461699</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J14" s="3">
-        <v>0.73749999999999993</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="K14" s="3">
-        <v>1.7661258578300369E-2</v>
+        <v>4.1503790974616983E-2</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.35">
@@ -3730,37 +3743,37 @@
         <v>68</v>
       </c>
       <c r="B15" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3">
-        <v>0.85011982917785645</v>
+        <v>0.86907339096069336</v>
       </c>
       <c r="E15" s="3">
-        <v>0.72332215309143066</v>
+        <v>0.72780632972717285</v>
       </c>
       <c r="F15" s="3">
-        <v>0.68765206038951865</v>
+        <v>0.68899188439051307</v>
       </c>
       <c r="G15" s="3">
-        <v>0.78617161512374878</v>
+        <v>0.77105879783630371</v>
       </c>
       <c r="H15" s="3">
-        <v>0.73676198959350581</v>
+        <v>0.74199705123901372</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J15" s="3">
-        <v>0.70999999999999985</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="K15" s="3">
-        <v>2.6761989593505949E-2</v>
+        <v>1.0029487609862771E-3</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.35">
@@ -3768,37 +3781,37 @@
         <v>69</v>
       </c>
       <c r="B16" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3">
-        <v>0.86907339096069336</v>
+        <v>0.85011982917785645</v>
       </c>
       <c r="E16" s="3">
-        <v>0.72780632972717285</v>
+        <v>0.72332215309143066</v>
       </c>
       <c r="F16" s="3">
-        <v>0.68899188439051307</v>
+        <v>0.68765206038951865</v>
       </c>
       <c r="G16" s="3">
-        <v>0.77105879783630371</v>
+        <v>0.78617161512374878</v>
       </c>
       <c r="H16" s="3">
-        <v>0.74199705123901372</v>
+        <v>0.73676198959350581</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J16" s="3">
-        <v>0.74299999999999999</v>
+        <v>0.70999999999999985</v>
       </c>
       <c r="K16" s="3">
-        <v>1.0029487609862771E-3</v>
+        <v>2.6761989593505949E-2</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
@@ -3846,7 +3859,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="3">
-        <v>0.75709245509334988</v>
+        <v>0.75709245509334977</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
@@ -3902,7 +3915,7 @@
         <v>26</v>
       </c>
       <c r="B10" s="3">
-        <v>4.4914704722970822E-2</v>
+        <v>4.4914704722970808E-2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
@@ -3910,7 +3923,7 @@
         <v>27</v>
       </c>
       <c r="B11" s="3">
-        <v>0.63718105832317884</v>
+        <v>0.63718105832317895</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
@@ -3958,7 +3971,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4029,13 +4044,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView zoomScale="106" zoomScaleNormal="106" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="39.6328125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.90625" customWidth="1"/>
     <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.26953125" bestFit="1" customWidth="1"/>
@@ -4055,7 +4073,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
     </row>
-    <row r="2" spans="1:10" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>40</v>
       </c>
@@ -4071,7 +4089,7 @@
       <c r="E2" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="7" t="s">
         <v>45</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -4092,57 +4110,57 @@
         <v>50</v>
       </c>
       <c r="B3" s="3">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="C3" s="3">
-        <v>20</v>
+        <v>101</v>
       </c>
       <c r="D3" s="3">
-        <v>0.68509304702281959</v>
+        <v>1.000000027418136</v>
       </c>
       <c r="E3" s="3">
-        <v>0.76250000000000007</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4">
-        <v>7.7406952977180477E-2</v>
+        <v>2.7418136427925791E-8</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>51</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="J3" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="3">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.68509304702281959</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.76250000000000007</v>
+      </c>
+      <c r="F4" s="4">
+        <v>7.7406952977180477E-2</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B4" s="3">
-        <v>23</v>
-      </c>
-      <c r="C4" s="3">
-        <v>24</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0.75970676183700558</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.78250000000000008</v>
-      </c>
-      <c r="F4" s="4">
-        <v>2.27932381629945E-2</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>56</v>
@@ -4156,25 +4174,25 @@
         <v>58</v>
       </c>
       <c r="B5" s="3">
-        <v>100</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3">
-        <v>101</v>
+        <v>22</v>
       </c>
       <c r="D5" s="3">
-        <v>1.000000027418136</v>
+        <v>0.68147463917732243</v>
       </c>
       <c r="E5" s="3">
-        <v>1</v>
+        <v>0.78</v>
       </c>
       <c r="F5" s="4">
-        <v>2.7418136427925791E-8</v>
+        <v>9.8525360822677599E-2</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>56</v>
@@ -4188,31 +4206,31 @@
         <v>59</v>
       </c>
       <c r="B6" s="3">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3">
-        <v>0.68147463917732243</v>
+        <v>0.75970676183700558</v>
       </c>
       <c r="E6" s="3">
-        <v>0.78</v>
+        <v>0.78250000000000008</v>
       </c>
       <c r="F6" s="4">
-        <v>9.8525360822677599E-2</v>
+        <v>2.27932381629945E-2</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>51</v>
       </c>
       <c r="H6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="J6" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -4220,31 +4238,31 @@
         <v>60</v>
       </c>
       <c r="B7" s="3">
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C7" s="3">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="D7" s="3">
-        <v>0.75292744398117062</v>
+        <v>0.77654744505882256</v>
       </c>
       <c r="E7" s="3">
-        <v>0.79549999999999998</v>
+        <v>0.71499999999999997</v>
       </c>
       <c r="F7" s="4">
-        <v>4.2572556018829373E-2</v>
+        <v>6.1547445058822592E-2</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I7" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J7" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
@@ -4252,31 +4270,31 @@
         <v>61</v>
       </c>
       <c r="B8" s="3">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="C8" s="3">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="D8" s="3">
-        <v>0.77654744505882256</v>
+        <v>0.74033935010433194</v>
       </c>
       <c r="E8" s="3">
-        <v>0.71499999999999997</v>
+        <v>0.78500000000000003</v>
       </c>
       <c r="F8" s="4">
-        <v>6.1547445058822592E-2</v>
+        <v>4.4660649895668092E-2</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J8" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
@@ -4284,31 +4302,31 @@
         <v>62</v>
       </c>
       <c r="B9" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D9" s="3">
-        <v>0.74033935010433194</v>
+        <v>0.75292744398117062</v>
       </c>
       <c r="E9" s="3">
-        <v>0.78500000000000003</v>
+        <v>0.79549999999999998</v>
       </c>
       <c r="F9" s="4">
-        <v>4.4660649895668092E-2</v>
+        <v>4.2572556018829373E-2</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J9" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -4316,31 +4334,31 @@
         <v>63</v>
       </c>
       <c r="B10" s="3">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C10" s="3">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D10" s="3">
-        <v>0.75246476262807849</v>
+        <v>0.68647099554538726</v>
       </c>
       <c r="E10" s="3">
-        <v>0.755</v>
+        <v>0.64749999999999996</v>
       </c>
       <c r="F10" s="4">
-        <v>2.5352373719215171E-3</v>
+        <v>3.8970995545387299E-2</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H10" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J10" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
@@ -4348,31 +4366,31 @@
         <v>64</v>
       </c>
       <c r="B11" s="3">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C11" s="3">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D11" s="3">
-        <v>0.80050379097461699</v>
+        <v>0.76516832530498502</v>
       </c>
       <c r="E11" s="3">
-        <v>0.75900000000000001</v>
+        <v>0.77749999999999997</v>
       </c>
       <c r="F11" s="4">
-        <v>4.1503790974616983E-2</v>
+        <v>1.2331674695014949E-2</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J11" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.35">
@@ -4380,19 +4398,19 @@
         <v>65</v>
       </c>
       <c r="B12" s="3">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C12" s="3">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D12" s="3">
-        <v>0.68647099554538726</v>
+        <v>0.75246476262807849</v>
       </c>
       <c r="E12" s="3">
-        <v>0.64749999999999996</v>
+        <v>0.755</v>
       </c>
       <c r="F12" s="4">
-        <v>3.8970995545387299E-2</v>
+        <v>2.5352373719215171E-3</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>51</v>
@@ -4401,10 +4419,10 @@
         <v>51</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
@@ -4412,31 +4430,31 @@
         <v>66</v>
       </c>
       <c r="B13" s="3">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C13" s="3">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D13" s="3">
-        <v>0.76516832530498502</v>
+        <v>0.71983874142169957</v>
       </c>
       <c r="E13" s="3">
-        <v>0.77749999999999997</v>
+        <v>0.73749999999999993</v>
       </c>
       <c r="F13" s="4">
-        <v>1.2331674695014949E-2</v>
+        <v>1.7661258578300369E-2</v>
       </c>
       <c r="G13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J13" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
@@ -4444,31 +4462,31 @@
         <v>67</v>
       </c>
       <c r="B14" s="3">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" s="3">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="D14" s="3">
-        <v>0.71983874142169957</v>
+        <v>0.80050379097461699</v>
       </c>
       <c r="E14" s="3">
-        <v>0.73749999999999993</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="F14" s="4">
-        <v>1.7661258578300369E-2</v>
+        <v>4.1503790974616983E-2</v>
       </c>
       <c r="G14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H14" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J14" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
@@ -4476,31 +4494,31 @@
         <v>68</v>
       </c>
       <c r="B15" s="3">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C15" s="3">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="3">
-        <v>0.73676198959350581</v>
+        <v>0.74199705123901372</v>
       </c>
       <c r="E15" s="3">
-        <v>0.70999999999999985</v>
+        <v>0.74299999999999999</v>
       </c>
       <c r="F15" s="4">
-        <v>2.6761989593505949E-2</v>
+        <v>1.0029487609862771E-3</v>
       </c>
       <c r="G15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H15" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J15" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
@@ -4508,31 +4526,31 @@
         <v>69</v>
       </c>
       <c r="B16" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C16" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="D16" s="3">
-        <v>0.74199705123901372</v>
+        <v>0.73676198959350581</v>
       </c>
       <c r="E16" s="3">
-        <v>0.74299999999999999</v>
+        <v>0.70999999999999985</v>
       </c>
       <c r="F16" s="4">
-        <v>1.0029487609862771E-3</v>
+        <v>2.6761989593505949E-2</v>
       </c>
       <c r="G16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>56</v>
-      </c>
       <c r="J16" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
@@ -4568,7 +4586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A12" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -4763,11 +4781,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="18.5" x14ac:dyDescent="0.35">
@@ -4826,7 +4851,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B3" s="3">
         <v>19</v>
@@ -4835,7 +4860,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E3" s="3">
         <v>0.68509304702281959</v>
@@ -4864,7 +4889,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B4" s="3">
         <v>21</v>
@@ -4873,7 +4898,7 @@
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E4" s="3">
         <v>0.68147463917732243</v>
@@ -4927,7 +4952,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -4965,7 +4992,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B4" s="3">
         <v>2</v>
@@ -4998,7 +5025,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>

</xml_diff>